<commit_message>
add to cart order completed
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Order/add_to_cart_order_test_data.xlsx
+++ b/TestData/Web_POS/Order/add_to_cart_order_test_data.xlsx
@@ -138,46 +138,55 @@
     <t>ATC_10</t>
   </si>
   <si>
+    <t>ATC_11</t>
+  </si>
+  <si>
+    <t>ATC_12</t>
+  </si>
+  <si>
+    <t>ATC_13</t>
+  </si>
+  <si>
     <t>Alexa67 : 1.8</t>
   </si>
   <si>
-    <t>ATC_11</t>
+    <t>ATC_14</t>
   </si>
   <si>
     <t>Alexa67 : 1.9</t>
   </si>
   <si>
-    <t>ATC_12</t>
+    <t>ATC_15</t>
   </si>
   <si>
     <t>Alexa67 : 1.10</t>
   </si>
   <si>
-    <t>ATC_13</t>
+    <t>ATC_16</t>
   </si>
   <si>
     <t>Alexa67 : 1.11</t>
   </si>
   <si>
-    <t>TC_32</t>
+    <t>ATC_17</t>
   </si>
   <si>
     <t>Alexa67 : 1.12</t>
   </si>
   <si>
-    <t>TC_33</t>
+    <t>ATC_18</t>
   </si>
   <si>
     <t>Alexa67 : 1.13</t>
   </si>
   <si>
-    <t>TC_34</t>
-  </si>
-  <si>
-    <t>TC_35</t>
-  </si>
-  <si>
-    <t>TC_36</t>
+    <t>ATC_19</t>
+  </si>
+  <si>
+    <t>ATC_20</t>
+  </si>
+  <si>
+    <t>ATC_21</t>
   </si>
 </sst>
 </file>
@@ -225,8 +234,25 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border/>
+    <border>
+      <left>
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="64"/>
+      </right>
+      <top>
+        <color indexed="64"/>
+      </top>
+      <bottom>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal>
+        <color indexed="64"/>
+      </diagonal>
+    </border>
     <border>
       <right style="medium">
         <color rgb="FF2B579A"/>
@@ -239,16 +265,24 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -472,8 +506,8 @@
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A11">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
@@ -1006,7 +1040,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" ht="14.25">
+    <row r="11" ht="28.5" customHeight="1">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1029,13 +1063,13 @@
         <v>1000</v>
       </c>
       <c r="H11">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>22</v>
@@ -1056,9 +1090,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" ht="14.25">
+    <row r="12" ht="28.5" customHeight="1">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
@@ -1079,13 +1113,13 @@
         <v>1000</v>
       </c>
       <c r="H12">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>22</v>
@@ -1106,9 +1140,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" ht="14.25">
+    <row r="13" ht="28.5" customHeight="1">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1129,13 +1163,13 @@
         <v>1000</v>
       </c>
       <c r="H13">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>22</v>
@@ -1156,150 +1190,150 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" ht="14.25">
+    <row r="14" ht="28.5" customHeight="1">
       <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G14">
+      <c r="D14" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="4">
+        <v>123456</v>
+      </c>
+      <c r="G14" s="5">
         <v>1000</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>600</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="3">
+      <c r="J14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="7">
         <v>45384</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="N14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" ht="14.25">
+    <row r="15" ht="28.5" customHeight="1">
       <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="4">
+        <v>123456</v>
+      </c>
+      <c r="G15" s="5">
         <v>1000</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>600</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="3">
+      <c r="J15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="7">
         <v>45384</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O15" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" ht="14.25">
+    <row r="16" ht="28.5" customHeight="1">
       <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G16">
+      <c r="D16" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="4">
+        <v>123456</v>
+      </c>
+      <c r="G16" s="5">
         <v>1000</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="5">
         <v>600</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="3">
+      <c r="J16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="7">
         <v>45384</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="N16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="O16" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P16" t="s">
@@ -1308,48 +1342,48 @@
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G17">
+      <c r="D17" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="4">
+        <v>123456</v>
+      </c>
+      <c r="G17" s="5">
         <v>1000</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="5">
         <v>600</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="3">
+      <c r="J17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="7">
         <v>45384</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="M17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="N17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="O17" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P17" t="s">
@@ -1358,48 +1392,48 @@
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G18">
+      <c r="F18" s="4">
+        <v>123456</v>
+      </c>
+      <c r="G18" s="5">
         <v>1000</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <v>600</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="3">
+      <c r="J18" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="7">
         <v>45384</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="M18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N18" s="3" t="s">
+      <c r="N18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="O18" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P18" t="s">
@@ -1408,48 +1442,48 @@
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="4">
+        <v>123456</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H19" s="5">
+        <v>600</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G19">
-        <v>1000</v>
-      </c>
-      <c r="H19">
-        <v>600</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="3">
+      <c r="K19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="7">
         <v>45384</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="M19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="N19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="O19" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P19" t="s">
@@ -1457,40 +1491,154 @@
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="I20" s="1"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="4">
+        <v>123456</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H20" s="5">
+        <v>600</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="7">
+        <v>45384</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="I21" s="1"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="4">
+        <v>123456</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H21" s="5">
+        <v>600</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="7">
+        <v>45384</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="I22" s="1"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="4">
+        <v>123456</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H22" s="5">
+        <v>600</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="7">
+        <v>45384</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P22" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" ht="14.25">
       <c r="B23" s="2"/>
@@ -1515,10 +1663,6 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="5"/>
     </row>
     <row r="25" ht="14.25">
       <c r="B25" s="2"/>
@@ -1568,140 +1712,122 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" ht="12.75">
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="5"/>
-    </row>
-    <row r="30" ht="12.75">
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="5"/>
-    </row>
-    <row r="31" ht="12.75">
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="5"/>
-    </row>
-    <row r="32" ht="12.75">
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="5"/>
-    </row>
-    <row r="33" ht="12.75">
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="5"/>
-    </row>
-    <row r="34" ht="12.75">
-      <c r="U34" s="1"/>
+    <row r="29" ht="14.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="I29" s="1"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="I30" s="1"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="9"/>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="I31" s="1"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="I32" s="1"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="I33" s="1"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="I34" s="1"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
     </row>
     <row r="35" ht="12.75">
-      <c r="U35" s="1"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="9"/>
     </row>
     <row r="36" ht="12.75">
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="5"/>
-    </row>
-    <row r="38" ht="14.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="I38" s="1"/>
-      <c r="K38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
-      <c r="U38" s="5"/>
-    </row>
-    <row r="39" ht="14.25">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="I39" s="1"/>
-      <c r="K39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-    </row>
-    <row r="40" ht="14.25">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="I40" s="1"/>
-      <c r="K40" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-    </row>
-    <row r="41" ht="14.25">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="I41" s="1"/>
-      <c r="K41" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-    </row>
-    <row r="42" ht="14.25">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="I42" s="1"/>
-      <c r="K42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-    </row>
-    <row r="43" ht="14.25">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="I43" s="1"/>
-      <c r="K43" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="9"/>
+    </row>
+    <row r="37" ht="12.75">
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="9"/>
+    </row>
+    <row r="38" ht="12.75">
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="9"/>
+    </row>
+    <row r="39" ht="12.75">
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="9"/>
+    </row>
+    <row r="40" ht="12.75">
+      <c r="U40" s="1"/>
+    </row>
+    <row r="41" ht="12.75">
+      <c r="U41" s="1"/>
+    </row>
+    <row r="42" ht="12.75">
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="9"/>
     </row>
     <row r="44" ht="14.25">
       <c r="B44" s="2"/>
@@ -1717,6 +1843,10 @@
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="9"/>
     </row>
     <row r="45" ht="14.25">
       <c r="B45" s="2"/>
@@ -1770,7 +1900,9 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="I48" s="1"/>
-      <c r="K48" s="1"/>
+      <c r="K48" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -1783,7 +1915,9 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="I49" s="1"/>
-      <c r="K49" s="1"/>
+      <c r="K49" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -1796,7 +1930,9 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="I50" s="1"/>
-      <c r="K50" s="1"/>
+      <c r="K50" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
@@ -1809,7 +1945,9 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="I51" s="1"/>
-      <c r="K51" s="1"/>
+      <c r="K51" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -1822,7 +1960,9 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="I52" s="1"/>
-      <c r="K52" s="1"/>
+      <c r="K52" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
@@ -1835,7 +1975,9 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="I53" s="1"/>
-      <c r="K53" s="1"/>
+      <c r="K53" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
@@ -1971,47 +2113,119 @@
       <c r="N63" s="3"/>
       <c r="O63" s="3"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="J64"/>
-      <c r="K64"/>
-      <c r="L64"/>
-    </row>
-    <row r="65" ht="12.75">
-      <c r="J65"/>
-      <c r="K65"/>
-      <c r="L65"/>
-    </row>
-    <row r="66" ht="12.75">
-      <c r="J66"/>
-      <c r="K66"/>
-      <c r="L66"/>
-    </row>
-    <row r="67" ht="12.75">
-      <c r="J67"/>
-      <c r="K67"/>
-      <c r="L67"/>
-    </row>
-    <row r="68" ht="12.75">
-      <c r="J68"/>
-      <c r="K68"/>
-      <c r="L68"/>
-    </row>
-    <row r="69" ht="12.75">
-      <c r="J69"/>
-      <c r="K69"/>
-      <c r="L69"/>
-    </row>
-    <row r="70" ht="12.75">
+    <row r="64" ht="14.25">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="I64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+    </row>
+    <row r="65" ht="14.25">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="I65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+    </row>
+    <row r="66" ht="14.25">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="I66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+    </row>
+    <row r="67" ht="14.25">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="I67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+    </row>
+    <row r="68" ht="14.25">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="I68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+    </row>
+    <row r="69" ht="14.25">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="I69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
       <c r="J70"/>
       <c r="K70"/>
       <c r="L70"/>
     </row>
-    <row r="71" ht="12.75"/>
-    <row r="72" ht="12.75"/>
-    <row r="73" ht="12.75"/>
-    <row r="74" ht="12.75"/>
-    <row r="75" ht="12.75"/>
-    <row r="76" ht="12.75"/>
+    <row r="71" ht="12.75">
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+    </row>
+    <row r="72" ht="12.75">
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="L72"/>
+    </row>
+    <row r="73" ht="12.75">
+      <c r="J73"/>
+      <c r="K73"/>
+      <c r="L73"/>
+    </row>
+    <row r="74" ht="12.75">
+      <c r="J74"/>
+      <c r="K74"/>
+      <c r="L74"/>
+    </row>
+    <row r="75" ht="12.75">
+      <c r="J75"/>
+      <c r="K75"/>
+      <c r="L75"/>
+    </row>
+    <row r="76" ht="12.75">
+      <c r="J76"/>
+      <c r="K76"/>
+      <c r="L76"/>
+    </row>
     <row r="77" ht="12.75"/>
     <row r="78" ht="12.75"/>
     <row r="79" ht="12.75"/>
@@ -2036,6 +2250,12 @@
     <row r="98" ht="12.75"/>
     <row r="99" ht="12.75"/>
     <row r="100" ht="12.75"/>
+    <row r="101" ht="12.75"/>
+    <row r="102" ht="12.75"/>
+    <row r="103" ht="12.75"/>
+    <row r="104" ht="12.75"/>
+    <row r="105" ht="12.75"/>
+    <row r="106" ht="12.75"/>
   </sheetData>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>